<commit_message>
Annuity calculaton and sensitivity analysis
</commit_message>
<xml_diff>
--- a/spårväxel_LCC/data_sc_LCC.xlsx
+++ b/spårväxel_LCC/data_sc_LCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\mistra-inframaint\spårväxel_LCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80577068-21EC-4B0E-A9AF-EB813798F69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AB2AC5-C009-4FC5-B9DA-D23D72D67AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prev" sheetId="1" r:id="rId1"/>
@@ -7613,7 +7613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8A562B-CFBD-489E-A647-0E7CEEE56D87}">
   <dimension ref="A1:J229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+    <sheetView topLeftCell="A133" workbookViewId="0">
       <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
@@ -13900,8 +13900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96BBDD0-6065-4C41-85E6-BFC7373BCA91}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13961,7 +13961,7 @@
         <v>30.66188</v>
       </c>
       <c r="G2" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H2" s="10">
         <v>550</v>
@@ -13991,7 +13991,7 @@
         <v>72.945830000000001</v>
       </c>
       <c r="G3" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H3">
         <v>550</v>
@@ -14021,7 +14021,7 @@
         <v>18.537410000000001</v>
       </c>
       <c r="G4" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H4">
         <v>350</v>
@@ -14051,7 +14051,7 @@
         <v>38.25403</v>
       </c>
       <c r="G5" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H5">
         <v>250</v>
@@ -14088,7 +14088,7 @@
         <v>74.416460000000001</v>
       </c>
       <c r="G6" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H6" s="11">
         <v>550</v>
@@ -14125,7 +14125,7 @@
         <v>82.305750000000003</v>
       </c>
       <c r="G7" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H7" s="11">
         <v>550</v>
@@ -14155,7 +14155,7 @@
         <v>19.991150000000001</v>
       </c>
       <c r="G8" s="9">
-        <v>6500000</v>
+        <v>4500000</v>
       </c>
       <c r="H8">
         <v>450</v>

</xml_diff>

<commit_message>
Preliminary results for ERS
</commit_message>
<xml_diff>
--- a/spårväxel_LCC/data_sc_LCC.xlsx
+++ b/spårväxel_LCC/data_sc_LCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\mistra-inframaint\spårväxel_LCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AB2AC5-C009-4FC5-B9DA-D23D72D67AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916C8E45-6072-44AA-B414-0E8B065B429D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prev" sheetId="1" r:id="rId1"/>
@@ -505,9 +505,9 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -533,7 +533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>1</v>
@@ -602,7 +602,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -637,7 +637,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -672,7 +672,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -707,7 +707,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -742,7 +742,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -777,7 +777,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -812,7 +812,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -847,7 +847,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -882,7 +882,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -917,7 +917,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -952,7 +952,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -987,7 +987,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1022,7 +1022,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1057,7 +1057,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1092,7 +1092,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1127,7 +1127,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1162,7 +1162,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1197,7 +1197,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1232,7 +1232,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1267,7 +1267,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1302,7 +1302,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1337,7 +1337,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1372,7 +1372,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1407,7 +1407,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1442,7 +1442,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1477,7 +1477,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1512,7 +1512,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1547,7 +1547,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1582,7 +1582,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1617,7 +1617,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1652,7 +1652,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1687,7 +1687,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1722,7 +1722,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1757,7 +1757,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1792,7 +1792,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1827,7 +1827,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1862,7 +1862,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1897,7 +1897,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1932,7 +1932,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1967,7 +1967,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2002,7 +2002,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2037,7 +2037,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2072,7 +2072,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2107,7 +2107,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2142,7 +2142,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2177,7 +2177,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2212,7 +2212,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2247,7 +2247,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2282,7 +2282,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2317,7 +2317,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2352,7 +2352,7 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2387,7 +2387,7 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2422,7 +2422,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2457,7 +2457,7 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -2492,7 +2492,7 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2527,7 +2527,7 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2562,7 +2562,7 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2597,7 +2597,7 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2632,7 +2632,7 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2667,7 +2667,7 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2702,7 +2702,7 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2737,7 +2737,7 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2772,7 +2772,7 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2807,7 +2807,7 @@
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A77" si="1">A66+1</f>
         <v>65</v>
@@ -2842,7 +2842,7 @@
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -2877,7 +2877,7 @@
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -2912,7 +2912,7 @@
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -2947,7 +2947,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -2982,7 +2982,7 @@
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -3017,7 +3017,7 @@
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -3052,7 +3052,7 @@
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3087,7 +3087,7 @@
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -3122,7 +3122,7 @@
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -3157,7 +3157,7 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -3205,9 +3205,9 @@
       <selection activeCell="A77" sqref="A1:A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3262,7 +3262,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>1</v>
@@ -3292,7 +3292,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3322,7 +3322,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3352,7 +3352,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3382,7 +3382,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3412,7 +3412,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3442,7 +3442,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3472,7 +3472,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3502,7 +3502,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3532,7 +3532,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3562,7 +3562,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3592,7 +3592,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3622,7 +3622,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3652,7 +3652,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3682,7 +3682,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3712,7 +3712,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3742,7 +3742,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3772,7 +3772,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3802,7 +3802,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3832,7 +3832,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3862,7 +3862,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3892,7 +3892,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3922,7 +3922,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3952,7 +3952,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3982,7 +3982,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4012,7 +4012,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4042,7 +4042,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4072,7 +4072,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4102,7 +4102,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4132,7 +4132,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4162,7 +4162,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4192,7 +4192,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4222,7 +4222,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4252,7 +4252,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4282,7 +4282,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4312,7 +4312,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4342,7 +4342,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -4372,7 +4372,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -4402,7 +4402,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -4432,7 +4432,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -4462,7 +4462,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -4492,7 +4492,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -4522,7 +4522,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -4552,7 +4552,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -4582,7 +4582,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4612,7 +4612,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4642,7 +4642,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4672,7 +4672,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4702,7 +4702,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4732,7 +4732,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4762,7 +4762,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -4792,7 +4792,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -4822,7 +4822,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -4852,7 +4852,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -4882,7 +4882,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -4912,7 +4912,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -4942,7 +4942,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -4972,7 +4972,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -5002,7 +5002,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -5032,7 +5032,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -5062,7 +5062,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -5092,7 +5092,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -5122,7 +5122,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -5152,7 +5152,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -5182,7 +5182,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A77" si="1">A66+1</f>
         <v>65</v>
@@ -5212,7 +5212,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -5242,7 +5242,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -5272,7 +5272,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -5302,7 +5302,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -5332,7 +5332,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -5362,7 +5362,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -5392,7 +5392,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -5422,7 +5422,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -5452,7 +5452,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -5482,7 +5482,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -5525,9 +5525,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>1</v>
@@ -5606,7 +5606,7 @@
         <v>0.11188326359763512</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5633,7 +5633,7 @@
         <v>0.24309534075671391</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5660,7 +5660,7 @@
         <v>0.38275046779629196</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5687,7 +5687,7 @@
         <v>0.52818753044375766</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5714,7 +5714,7 @@
         <v>0.67808106497878928</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5741,7 +5741,7 @@
         <v>0.8316244306954409</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5768,7 +5768,7 @@
         <v>0.98827098432979998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5795,7 +5795,7 @@
         <v>1.1476240821722545</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5822,7 +5822,7 @@
         <v>1.3093819029549374</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5849,7 +5849,7 @@
         <v>1.4733065719686291</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5876,7 +5876,7 @@
         <v>1.6392054757038956</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5903,7 +5903,7 @@
         <v>1.8069192644268695</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5930,7 +5930,7 @@
         <v>1.9763137828449826</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5957,7 +5957,7 @@
         <v>2.1472744356082929</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5984,7 +5984,7 @@
         <v>2.3197021295142601</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6011,7 +6011,7 @@
         <v>2.4935102744193838</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6038,7 +6038,7 @@
         <v>2.6686225171100908</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6065,7 +6065,7 @@
         <v>2.8449709960572958</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6092,7 +6092,7 @@
         <v>3.0224949748148191</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6119,7 +6119,7 @@
         <v>3.201139756164479</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6146,7 +6146,7 @@
         <v>3.3808558080864599</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6173,7 +6173,7 @@
         <v>3.5615980520515724</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6200,7 +6200,7 @@
         <v>3.7433252774393035</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6227,7 +6227,7 @@
         <v>3.9259996551888703</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6254,7 +6254,7 @@
         <v>4.1095863304124043</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6281,7 +6281,7 @@
         <v>4.2940530784896271</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6308,7 +6308,7 @@
         <v>4.479370012679845</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6335,7 +6335,7 @@
         <v>4.6655093339037359</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6362,7 +6362,7 @@
         <v>4.8524451153180204</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6389,7 +6389,7 @@
         <v>5.0401531158076045</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -6416,7 +6416,7 @@
         <v>5.2286106176754323</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -6443,7 +6443,7 @@
         <v>5.4177962847086611</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -6470,7 +6470,7 @@
         <v>5.6076900375041525</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -6497,7 +6497,7 @@
         <v>5.7982729434934832</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -6524,7 +6524,7 @@
         <v>5.9895271195517008</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -6551,7 +6551,7 @@
         <v>6.1814356454304793</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -6578,7 +6578,7 @@
         <v>6.3739824865444934</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -6605,7 +6605,7 @@
         <v>6.5671524248743349</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -6632,7 +6632,7 @@
         <v>6.7609309969410436</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -6659,7 +6659,7 @@
         <v>6.955304437965256</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -6686,7 +6686,7 @@
         <v>7.1502596314548637</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -6713,7 +6713,7 @@
         <v>7.3457840635734293</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -6740,7 +6740,7 @@
         <v>7.5418657817328523</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -6767,7 +6767,7 @@
         <v>7.7384933569298031</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6794,7 +6794,7 @@
         <v>7.9356558494098497</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -6821,7 +6821,7 @@
         <v>8.13334277729777</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -6848,7 +6848,7 @@
         <v>8.3315440878786617</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -6875,7 +6875,7 @@
         <v>8.5302501312542383</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -6902,7 +6902,7 @@
         <v>8.7294516361322518</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -6929,7 +6929,7 @@
         <v>8.9291396875363738</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -6956,7 +6956,7 @@
         <v>9.1293057062485854</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -6983,7 +6983,7 @@
         <v>9.3299414298182555</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -7010,7 +7010,7 @@
         <v>9.531038894990381</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -7037,7 +7037,7 @@
         <v>9.7325904214223264</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -7064,7 +7064,7 @@
         <v>9.9345885965723202</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -7091,7 +7091,7 @@
         <v>10.137026261655558</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -7118,7 +7118,7 @@
         <v>10.339896498574845</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -7145,7 +7145,7 @@
         <v>10.543192617742156</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -7172,7 +7172,7 @@
         <v>10.746908146715981</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -7199,7 +7199,7 @@
         <v>10.951036819587021</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -7226,7 +7226,7 @@
         <v>11.155572567051211</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -7253,7 +7253,7 @@
         <v>11.36050950711495</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -7280,7 +7280,7 @@
         <v>11.565841936382835</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -7307,7 +7307,7 @@
         <v>11.771564321882618</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A77" si="1">A66+1</f>
         <v>65</v>
@@ -7334,7 +7334,7 @@
         <v>11.977671293386463</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -7361,7 +7361,7 @@
         <v>12.184157636191035</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -7388,7 +7388,7 @@
         <v>12.391018284322653</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -7415,7 +7415,7 @@
         <v>12.598248314136381</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -7442,7 +7442,7 @@
         <v>12.805842938280737</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -7469,7 +7469,7 @@
         <v>13.013797500002285</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -7496,7 +7496,7 @@
         <v>13.222107467766168</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -7523,7 +7523,7 @@
         <v>13.430768430171026</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -7550,7 +7550,7 @@
         <v>13.639776091138177</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -7577,7 +7577,7 @@
         <v>13.849126265356926</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -7617,12 +7617,12 @@
       <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>1</v>
@@ -7713,7 +7713,7 @@
         <v>0.38148730691159943</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -7743,7 +7743,7 @@
         <v>1.0716961748676079</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -7773,7 +7773,7 @@
         <v>1.9610151003140215</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7803,7 +7803,7 @@
         <v>3.0106707888239326</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7833,7 +7833,7 @@
         <v>4.1983390087089605</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7863,7 +7863,7 @@
         <v>5.5089968756186014</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7893,7 +7893,7 @@
         <v>6.9316383456221065</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7923,7 +7923,7 @@
         <v>8.4577502572475449</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7953,7 +7953,7 @@
         <v>10.080493253608394</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7983,7 +7983,7 @@
         <v>11.794216412745486</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8013,7 +8013,7 @@
         <v>13.594148711170909</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -8043,7 +8043,7 @@
         <v>15.476192187768291</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -8073,7 +8073,7 @@
         <v>17.436777372266153</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8103,7 +8103,7 @@
         <v>19.472758768066289</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8133,7 +8133,7 @@
         <v>21.581337158941118</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8163,7 +8163,7 @@
         <v>23.760000488766249</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8193,7 +8193,7 @@
         <v>26.006477968569992</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -8223,7 +8223,7 @@
         <v>28.318703833504564</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -8253,7 +8253,7 @@
         <v>30.694788288267333</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -8283,7 +8283,7 @@
         <v>33.132993905952077</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -8313,7 +8313,7 @@
         <v>35.631716231204805</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -8343,7 +8343,7 @@
         <v>38.189467671382474</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -8373,7 +8373,7 @@
         <v>40.804863992251775</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -8403,7 +8403,7 @@
         <v>43.476612900755306</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -8433,7 +8433,7 @@
         <v>46.203504317724914</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -8463,7 +8463,7 @@
         <v>48.984402032033941</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -8493,7 +8493,7 @@
         <v>51.81823649383027</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -8523,7 +8523,7 @@
         <v>54.703998554510726</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -8553,7 +8553,7 @@
         <v>57.64073399935188</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8583,7 +8583,7 @@
         <v>60.627538748294128</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -8613,7 +8613,7 @@
         <v>63.663554623466453</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -8643,7 +8643,7 @@
         <v>66.74796560023907</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -8673,7 +8673,7 @@
         <v>69.879994473048015</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -8703,7 +8703,7 @@
         <v>73.058899878819901</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -8733,7 +8733,7 @@
         <v>76.283973630167665</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -8763,7 +8763,7 @@
         <v>79.554538318120706</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -8793,7 +8793,7 @@
         <v>82.869945150359797</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -8823,7 +8823,7 @@
         <v>86.229571996034721</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -8853,7 +8853,7 @@
         <v>89.632821612466813</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8883,7 +8883,7 @@
         <v>93.079120032554201</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -8913,7 +8913,7 @@
         <v>96.567915094635524</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -8943,7 +8943,7 @@
         <v>100.09867509903566</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -8973,7 +8973,7 @@
         <v>103.67088757760324</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9003,7 +9003,7 @@
         <v>107.28405816431199</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9033,7 +9033,7 @@
         <v>110.93770955650321</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9063,7 +9063,7 @@
         <v>114.63138055763071</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9093,7 +9093,7 @@
         <v>118.36462519346966</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9123,7 +9123,7 @@
         <v>122.13701189470019</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9153,7 +9153,7 @@
         <v>125.94812273959261</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9183,7 +9183,7 @@
         <v>129.79755275123475</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -9213,7 +9213,7 @@
         <v>133.68490924435258</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -9243,7 +9243,7 @@
         <v>137.60981121731697</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -9273,7 +9273,7 @@
         <v>141.57188878539679</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -9303,7 +9303,7 @@
         <v>145.57078265173206</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -9333,7 +9333,7 @@
         <v>149.60614361285874</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -9363,7 +9363,7 @@
         <v>153.67763209594168</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -9393,7 +9393,7 @@
         <v>157.78491772514602</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -9423,7 +9423,7 @@
         <v>161.92767891483527</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -9453,7 +9453,7 @@
         <v>166.1056024874965</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -9483,7 +9483,7 @@
         <v>170.31838331449566</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -9513,7 +9513,7 @@
         <v>174.5657239779413</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -9543,7 +9543,7 @@
         <v>178.84733445208516</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -9573,7 +9573,7 @@
         <v>183.16293180283606</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -9603,7 +9603,7 @@
         <v>187.5122399040844</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A77" si="1">A66+1</f>
         <v>65</v>
@@ -9633,7 +9633,7 @@
         <v>191.8949891696457</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -9663,7 +9663,7 @@
         <v>196.31091629973719</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -9693,7 +9693,7 @@
         <v>200.75976404098972</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -9723,7 +9723,7 @@
         <v>205.24128095908125</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -9753,7 +9753,7 @@
         <v>209.75522122314842</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -9783,7 +9783,7 @@
         <v>214.30134440120858</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -9813,7 +9813,7 @@
         <v>218.87941526587542</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -9843,7 +9843,7 @@
         <v>223.48920360971562</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -9873,7 +9873,7 @@
         <v>228.13048406963654</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -9903,7 +9903,7 @@
         <v>232.80303595974971</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -9933,7 +9933,7 @@
         <v>237.50664311218708</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>0</v>
       </c>
@@ -9962,7 +9962,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>0.91528817044987221</v>
       </c>
@@ -9988,7 +9988,7 @@
         <v>0.68611068017489185</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>2.003503374780605</v>
       </c>
@@ -10014,7 +10014,7 @@
         <v>1.5018494803967279</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>3.1682042612455676</v>
       </c>
@@ -10040,7 +10040,7 @@
         <v>2.3749228393804929</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>4.3855322316515295</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>3.2874460738506124</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>5.6435531627854232</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>4.2304732259553806</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>6.9349830297489072</v>
       </c>
@@ -10118,7 +10118,7 @@
         <v>5.1985441057363104</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>8.2548744403964136</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>6.187950090379652</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>9.5996309249843677</v>
       </c>
@@ -10170,7 +10170,7 @@
         <v>7.1959952242490717</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>10.966511493359565</v>
       </c>
@@ -10196,7 +10196,7 @@
         <v>8.2206248291797213</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>12.35335293565187</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>9.2602173378409205</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89">
         <v>13.758401525903444</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>10.313458136815147</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90">
         <v>15.180204828080544</v>
       </c>
@@ -10274,7 +10274,7 @@
         <v>11.379258463123485</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91">
         <v>16.617538845022455</v>
       </c>
@@ -10300,7 +10300,7 @@
         <v>12.456700794228684</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92">
         <v>18.069357098317429</v>
       </c>
@@ -10326,7 +10326,7 @@
         <v>13.545000677716681</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93">
         <v>19.534753923580741</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>14.643479217009245</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94">
         <v>21.012937319403257</v>
       </c>
@@ -10378,7 +10378,7 @@
         <v>15.751542718619378</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95">
         <v>22.503208415862989</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>16.868667301508292</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>24.004945650851162</v>
       </c>
@@ -10430,7 +10430,7 @@
         <v>17.99438703547499</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>25.517592371049098</v>
       </c>
@@ -10456,7 +10456,7 @@
         <v>19.128284646704049</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98">
         <v>27.04064697380451</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>20.269984128001173</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99">
         <v>28.573654967327446</v>
       </c>
@@ -10508,7 +10508,7 @@
         <v>21.419144787023559</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100">
         <v>30.116202501760437</v>
       </c>
@@ -10534,7 +10534,7 @@
         <v>22.575456397094658</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B101">
         <v>31.667911043769678</v>
       </c>
@@ -10560,7 +10560,7 @@
         <v>23.738635205215676</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102">
         <v>33.228432951309379</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>24.908420614857352</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>34.797447765036615</v>
       </c>
@@ -10612,7 +10612,7 @@
         <v>26.084572405961303</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104">
         <v>36.374659076153407</v>
       </c>
@@ -10638,7 +10638,7 @@
         <v>27.266868387037942</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B105">
         <v>37.959791862253837</v>
       </c>
@@ -10664,7 +10664,7 @@
         <v>28.455102398086435</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>39.552590206427823</v>
       </c>
@@ -10690,7 +10690,7 @@
         <v>29.649082600808288</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>41.152815332711228</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>30.848630005957883</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B108">
         <v>42.760243904568377</v>
       </c>
@@ -10742,7 +10742,7 @@
         <v>32.053577197865096</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B109">
         <v>44.374666543562583</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>33.263767224013499</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B110">
         <v>45.995886533511609</v>
       </c>
@@ -10794,7 +10794,7 @@
         <v>34.479052623660188</v>
       </c>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>47.623718681811674</v>
       </c>
@@ -10820,7 +10820,7 @@
         <v>35.699294574270951</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B112">
         <v>49.257988314667088</v>
       </c>
@@ -10846,7 +10846,7 @@
         <v>36.924362138332746</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B113">
         <v>50.898530386990451</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>38.154131596124458</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B114">
         <v>52.545188690974456</v>
       </c>
@@ -10898,7 +10898,7 @@
         <v>39.388485852453151</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B115">
         <v>54.197815149951452</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>40.627313907322922</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B116">
         <v>55.85626918628752</v>
       </c>
@@ -10950,7 +10950,7 @@
         <v>41.870510382100981</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B117">
         <v>57.520417153798711</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>43.117975094050188</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B118">
         <v>59.190131826614049</v>
       </c>
@@ -11002,7 +11002,7 @@
         <v>44.369612673174856</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B119">
         <v>60.86529193759695</v>
       </c>
@@ -11028,7 +11028,7 @@
         <v>45.625332216216052</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B120">
         <v>62.545781760425804</v>
       </c>
@@ -11054,7 +11054,7 @@
         <v>46.885046973374315</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>64.231490730260077</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>48.148674063956541</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>65.922313098612975</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>49.41613421766457</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B123">
         <v>67.618147618637479</v>
       </c>
@@ -11132,7 +11132,7 @@
         <v>50.687351538681831</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>69.318897257527013</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>51.962253290085606</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B125">
         <v>71.024468933155802</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>53.240769696429545</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126">
         <v>72.734773272441672</v>
       </c>
@@ -11210,7 +11210,7 @@
         <v>54.522833762609636</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>74.449724389223917</v>
       </c>
@@ -11236,7 +11236,7 @@
         <v>55.808381107358812</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>76.169239679713371</v>
       </c>
@@ -11262,7 +11262,7 @@
         <v>57.097349809913958</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B129">
         <v>77.893239633799951</v>
       </c>
@@ -11288,7 +11288,7 @@
         <v>58.389680268569876</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>79.621647660700958</v>
       </c>
@@ -11314,7 +11314,7 @@
         <v>59.685315069983218</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B131">
         <v>81.354389927605155</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v>60.984198868218137</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>83.091395210116602</v>
       </c>
@@ -11366,7 +11366,7 @@
         <v>62.286278272637333</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>84.832594753431962</v>
       </c>
@@ -11392,7 +11392,7 @@
         <v>63.591501743838904</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>86.577922143299958</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>64.899819496926028</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B135">
         <v>88.327313185910782</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>66.211183411470699</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B136">
         <v>90.080705795951815</v>
       </c>
@@ -11470,7 +11470,7 @@
         <v>67.525546947598968</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B137">
         <v>91.838039892142376</v>
       </c>
@@ -11496,7 +11496,7 @@
         <v>68.842865067682638</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B138">
         <v>93.599257299629272</v>
       </c>
@@ -11522,7 +11522,7 @@
         <v>70.163094163173682</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B139">
         <v>95.364301658686884</v>
       </c>
@@ -11548,7 +11548,7 @@
         <v>71.48619198616494</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B140">
         <v>97.133118339215642</v>
       </c>
@@ -11574,7 +11574,7 @@
         <v>72.812117585297045</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B141">
         <v>98.905654360585061</v>
       </c>
@@ -11600,7 +11600,7 @@
         <v>74.140831245671933</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B142">
         <v>100.68185831640569</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>75.472294432460899</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B143">
         <v>102.46168030385601</v>
       </c>
@@ -11652,7 +11652,7 @@
         <v>76.806469737927316</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B144">
         <v>104.24507185722155</v>
       </c>
@@ -11678,7 +11678,7 @@
         <v>78.143320831606772</v>
       </c>
     </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B145">
         <v>106.03198588533583</v>
       </c>
@@ -11704,7 +11704,7 @@
         <v>79.482812413412034</v>
       </c>
     </row>
-    <row r="146" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B146">
         <v>107.82237661263869</v>
       </c>
@@ -11730,7 +11730,7 @@
         <v>80.824910169449694</v>
       </c>
     </row>
-    <row r="147" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B147">
         <v>109.61619952359207</v>
       </c>
@@ -11756,7 +11756,7 @@
         <v>82.169580730353587</v>
       </c>
     </row>
-    <row r="148" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B148">
         <v>111.41341131021814</v>
       </c>
@@ -11782,7 +11782,7 @@
         <v>83.516791631958796</v>
       </c>
     </row>
-    <row r="149" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B149">
         <v>113.21396982253944</v>
       </c>
@@ -11808,7 +11808,7 @@
         <v>84.866511278150938</v>
       </c>
     </row>
-    <row r="150" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B150">
         <v>115.01783402172423</v>
       </c>
@@ -11834,7 +11834,7 @@
         <v>86.218708905743455</v>
       </c>
     </row>
-    <row r="151" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B151">
         <v>116.82496393575178</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>87.573354551243725</v>
       </c>
     </row>
-    <row r="152" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B152">
         <v>118.63532061743192</v>
       </c>
@@ -11886,7 +11886,7 @@
         <v>88.93041901938409</v>
       </c>
     </row>
-    <row r="153" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B153">
         <v>120.44886610461968</v>
       </c>
@@ -11912,7 +11912,7 @@
         <v>90.289873853298232</v>
       </c>
     </row>
-    <row r="154" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B154">
         <v>0</v>
       </c>
@@ -11941,7 +11941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B155">
         <v>0.14787874957156202</v>
       </c>
@@ -11967,7 +11967,7 @@
         <v>0.11867547635036431</v>
       </c>
     </row>
-    <row r="156" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B156">
         <v>0.32130484812328519</v>
       </c>
@@ -11993,7 +11993,7 @@
         <v>0.25785318049541545</v>
       </c>
     </row>
-    <row r="157" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B157">
         <v>0.5058903249300859</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>0.4059864954637401</v>
       </c>
     </row>
-    <row r="158" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B158">
         <v>0.69811792246436766</v>
       </c>
@@ -12045,7 +12045,7 @@
         <v>0.56025275597216695</v>
       </c>
     </row>
-    <row r="159" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B159">
         <v>0.89623574405042605</v>
       </c>
@@ -12071,7 +12071,7 @@
         <v>0.71924603200635528</v>
       </c>
     </row>
-    <row r="160" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B160">
         <v>1.0991776336331627</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>0.88211071329052704</v>
       </c>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B161">
         <v>1.3062210799116933</v>
       </c>
@@ -12123,7 +12123,7 @@
         <v>1.0482669709239825</v>
       </c>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B162">
         <v>1.5168418295355455</v>
       </c>
@@ -12149,7 +12149,7 @@
         <v>1.2172940817380724</v>
       </c>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B163">
         <v>1.7306409582129965</v>
       </c>
@@ -12175,7 +12175,7 @@
         <v>1.3888719014897255</v>
       </c>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B164">
         <v>1.9473040613278159</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>1.5627481145642508</v>
       </c>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B165">
         <v>2.166576557059543</v>
       </c>
@@ -12227,7 +12227,7 @@
         <v>1.7387184142651091</v>
       </c>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B166">
         <v>2.3882478291047993</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>1.9166137770496818</v>
       </c>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B167">
         <v>2.6121405612477768</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>2.0962919033215996</v>
       </c>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B168">
         <v>2.8381032901103871</v>
       </c>
@@ -12305,7 +12305,7 @@
         <v>2.2776312408727426</v>
       </c>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B169">
         <v>3.0660050418685598</v>
       </c>
@@ -12331,7 +12331,7 @@
         <v>2.4605266807472548</v>
       </c>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B170">
         <v>3.2957313682863911</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>2.6448863760844286</v>
       </c>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B171">
         <v>3.5271813515198174</v>
       </c>
@@ -12383,7 +12383,7 @@
         <v>2.8306293384173533</v>
       </c>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B172">
         <v>3.7602652973845392</v>
       </c>
@@ -12409,7 +12409,7 @@
         <v>3.0176835864770615</v>
       </c>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B173">
         <v>3.9949029290864626</v>
       </c>
@@ -12435,7 +12435,7 @@
         <v>3.2059846966272514</v>
       </c>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B174">
         <v>4.2310219520216421</v>
       </c>
@@ -12461,7 +12461,7 @@
         <v>3.395474651089267</v>
       </c>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B175">
         <v>4.4685568985506974</v>
       </c>
@@ -12487,7 +12487,7 @@
         <v>3.586100910851846</v>
       </c>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B176">
         <v>4.7074481873178948</v>
       </c>
@@ -12513,7 +12513,7 @@
         <v>3.7778156607570041</v>
       </c>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B177">
         <v>4.9476413492736668</v>
       </c>
@@ -12539,7 +12539,7 @@
         <v>3.9705751883685569</v>
       </c>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B178">
         <v>5.1890863848557363</v>
       </c>
@@ -12565,7 +12565,7 @@
         <v>4.1643393680978873</v>
       </c>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B179">
         <v>5.4317372255363487</v>
       </c>
@@ -12591,7 +12591,7 @@
         <v>4.3590712290854778</v>
       </c>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B180">
         <v>5.6755512792744867</v>
       </c>
@@ -12617,7 +12617,7 @@
         <v>4.5547365904177672</v>
       </c>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B181">
         <v>5.9204890440597469</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>4.7513037509888507</v>
       </c>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B182">
         <v>6.1665137771930238</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>4.9487432240920075</v>
       </c>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B183">
         <v>6.4135912105537685</v>
       </c>
@@ -12695,7 +12695,7 @@
         <v>5.1470275089163264</v>
       </c>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B184">
         <v>6.6616893040881493</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>5.34613089271632</v>
       </c>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B185">
         <v>6.9107780312799045</v>
       </c>
@@ -12747,7 +12747,7 @@
         <v>5.5460292786482519</v>
       </c>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B186">
         <v>7.1608291915530584</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>5.7467000352197859</v>
       </c>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B187">
         <v>7.4118162454866736</v>
       </c>
@@ -12799,7 +12799,7 @@
         <v>5.9481218640467342</v>
       </c>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B188">
         <v>7.6637141694583208</v>
       </c>
@@ -12825,7 +12825,7 @@
         <v>6.1502746832017046</v>
       </c>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B189">
         <v>7.9164993269197668</v>
       </c>
@@ -12851,7 +12851,7 @@
         <v>6.3531395239104196</v>
       </c>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B190">
         <v>8.1701493539795358</v>
       </c>
@@ -12877,7 +12877,7 @@
         <v>6.5566984387295761</v>
       </c>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B191">
         <v>8.4246430573478435</v>
       </c>
@@ -12903,7 +12903,7 @@
         <v>6.7609344196457295</v>
       </c>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B192">
         <v>8.6799603230093396</v>
       </c>
@@ -12929,7 +12929,7 @@
         <v>6.9658313247834602</v>
       </c>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B193">
         <v>8.9360820342425953</v>
       </c>
@@ -12955,7 +12955,7 @@
         <v>7.1713738126144655</v>
       </c>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B194">
         <v>9.1929899978139211</v>
       </c>
@@ -12981,7 +12981,7 @@
         <v>7.3775472827267139</v>
       </c>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B195">
         <v>9.4506668773461922</v>
       </c>
@@ -13007,7 +13007,7 @@
         <v>7.5843378223516744</v>
       </c>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B196">
         <v>9.7090961330065042</v>
       </c>
@@ -13033,7 +13033,7 @@
         <v>7.7917321579625254</v>
       </c>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B197">
         <v>9.9682619667771206</v>
       </c>
@@ -13059,7 +13059,7 @@
         <v>7.9997176113530646</v>
       </c>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B198">
         <v>10.228149272674658</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>8.2082820596876633</v>
       </c>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B199">
         <v>10.488743591367539</v>
       </c>
@@ -13111,7 +13111,7 @@
         <v>8.4174138990809269</v>
       </c>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B200">
         <v>10.750031068713946</v>
       </c>
@@ -13137,7 +13137,7 @@
         <v>8.627102011323613</v>
       </c>
     </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B201">
         <v>11.011998417803383</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>8.837335733420284</v>
       </c>
     </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B202">
         <v>11.274632884137578</v>
       </c>
@@ -13189,7 +13189,7 @@
         <v>9.0481048296463182</v>
       </c>
     </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B203">
         <v>11.537922213630791</v>
       </c>
@@ -13215,7 +13215,7 @@
         <v>9.2593994658675598</v>
       </c>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B204">
         <v>11.801854623148452</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>9.4712101858970126</v>
       </c>
     </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B205">
         <v>12.066418773335661</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>9.6835278896892163</v>
       </c>
     </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B206">
         <v>12.331603743516451</v>
       </c>
@@ -13293,7 +13293,7 @@
         <v>9.8963438131964203</v>
       </c>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B207">
         <v>12.597399008468781</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>10.109649509730081</v>
       </c>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B208">
         <v>12.863794416902556</v>
       </c>
@@ -13345,7 +13345,7 @@
         <v>10.32343683268908</v>
       </c>
     </row>
-    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B209">
         <v>13.130780171486407</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>10.537697919530816</v>
       </c>
     </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B210">
         <v>13.398346810285531</v>
       </c>
@@ -13397,7 +13397,7 @@
         <v>10.75242517687475</v>
       </c>
     </row>
-    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B211">
         <v>13.666485189487627</v>
       </c>
@@ -13423,7 +13423,7 @@
         <v>10.967611266639622</v>
       </c>
     </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B212">
         <v>13.935186467306346</v>
       </c>
@@ -13449,7 +13449,7 @@
         <v>11.183249093125683</v>
       </c>
     </row>
-    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B213">
         <v>14.20444208896302</v>
       </c>
@@ -13475,7 +13475,7 @@
         <v>11.399331790962236</v>
       </c>
     </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B214">
         <v>14.474243772657468</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>11.615852713848959</v>
       </c>
     </row>
-    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B215">
         <v>14.744583496447296</v>
       </c>
@@ -13527,7 +13527,7 @@
         <v>11.832805424026279</v>
       </c>
     </row>
-    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B216">
         <v>15.015453485962764</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>12.050183682416343</v>
       </c>
     </row>
-    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B217">
         <v>15.286846202891589</v>
       </c>
@@ -13579,7 +13579,7 @@
         <v>12.267981439381835</v>
       </c>
     </row>
-    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B218">
         <v>15.558754334173791</v>
       </c>
@@ -13605,7 +13605,7 @@
         <v>12.48619282605465</v>
       </c>
     </row>
-    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B219">
         <v>15.831170781852515</v>
       </c>
@@ -13631,7 +13631,7 @@
         <v>12.704812146190989</v>
       </c>
     </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B220">
         <v>16.104088653531317</v>
       </c>
@@ -13657,7 +13657,7 @@
         <v>12.923833868513139</v>
       </c>
     </row>
-    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B221">
         <v>16.377501253393241</v>
       </c>
@@ -13683,7 +13683,7 @@
         <v>13.143252619502126</v>
       </c>
     </row>
-    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B222">
         <v>16.651402073740595</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v>13.363063176608222</v>
       </c>
     </row>
-    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B223">
         <v>16.925784787017964</v>
       </c>
@@ -13735,7 +13735,7 @@
         <v>13.583260461849257</v>
       </c>
     </row>
-    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B224">
         <v>17.200643238284439</v>
       </c>
@@ -13761,7 +13761,7 @@
         <v>13.803839535769457</v>
       </c>
     </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B225">
         <v>17.475971438103471</v>
       </c>
@@ -13787,7 +13787,7 @@
         <v>14.024795591733403</v>
       </c>
     </row>
-    <row r="226" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B226">
         <v>17.751763555821793</v>
       </c>
@@ -13813,7 +13813,7 @@
         <v>14.246123950532235</v>
       </c>
     </row>
-    <row r="227" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B227">
         <v>18.028013913210838</v>
       </c>
@@ -13839,7 +13839,7 @@
         <v>14.467820055280797</v>
       </c>
     </row>
-    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B228">
         <v>18.304716978446699</v>
       </c>
@@ -13865,7 +13865,7 @@
         <v>14.689879466586412</v>
       </c>
     </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B229">
         <v>18.581867360405756</v>
       </c>
@@ -13901,21 +13901,21 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -13941,7 +13941,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -13971,7 +13971,7 @@
         <v>68.75</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -14001,7 +14001,7 @@
         <v>68.75</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -14031,7 +14031,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -14068,7 +14068,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -14105,7 +14105,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -14135,7 +14135,7 @@
         <v>68.75</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -14165,22 +14165,22 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
     </row>
   </sheetData>

</xml_diff>